<commit_message>
add OH for m, ON for n, OB for ng
</commit_message>
<xml_diff>
--- a/TSP.xlsx
+++ b/TSP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tastror\OneDrive\桌面\TSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/156a5e04750dab24/桌面/TSP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDF079D-C59C-4818-B5BE-42665AE2A26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{84FDFF2F-C4A7-4E60-B612-76B73EDBDAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{427E4BFE-2EAF-4964-8938-08E6ECACBF23}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="149">
   <si>
     <t>韵母</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1654,10 +1654,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>aoeêɿʅ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>iü</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1670,8 +1666,24 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">i, </t>
+    <t>iau, ng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iou, n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>in, m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i, ɿ, ʅ, er</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>aoeê</t>
     </r>
     <r>
       <rPr>
@@ -1681,7 +1693,17 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>ɿ</t>
+      <t>ɿʅ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>m</t>
     </r>
     <r>
       <rPr>
@@ -1692,28 +1714,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>ʅ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, er</t>
+      <t>nng</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1722,7 +1723,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1906,6 +1907,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="1"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2506,6 +2514,10 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2771,7 +2783,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2801,7 +2815,7 @@
         <v>21</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K2" s="32" t="s">
         <v>131</v>
@@ -2831,7 +2845,7 @@
         <v>126</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
       <c r="I3" s="33" t="s">
         <v>42</v>
@@ -2853,7 +2867,7 @@
         <v>53</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>48</v>
@@ -2862,10 +2876,10 @@
         <v>125</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="I4" s="32" t="s">
         <v>56</v>
@@ -2994,7 +3008,7 @@
         <v>134</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>93</v>
@@ -3072,7 +3086,7 @@
         <v>137</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3098,7 +3112,7 @@
         <v>21</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K18" s="32" t="s">
         <v>131</v>
@@ -3123,8 +3137,8 @@
       <c r="F19" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>55</v>
+      <c r="H19" s="33" t="s">
+        <v>146</v>
       </c>
       <c r="I19" s="33" t="s">
         <v>42</v>
@@ -3142,7 +3156,7 @@
         <v>53</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>48</v>
@@ -3150,11 +3164,11 @@
       <c r="E20" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>46</v>
+      <c r="F20" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>145</v>
       </c>
       <c r="I20" s="32" t="s">
         <v>56</v>
@@ -3168,7 +3182,7 @@
         <v>139</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3194,7 +3208,7 @@
         <v>21</v>
       </c>
       <c r="J23" s="32" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K23" s="32" t="s">
         <v>131</v>
@@ -3220,7 +3234,7 @@
         <v>126</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>42</v>
@@ -3238,7 +3252,7 @@
         <v>53</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D25" s="28" t="s">
         <v>48</v>
@@ -3247,10 +3261,10 @@
         <v>125</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="H25" s="32" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="I25" s="9" t="s">
         <v>56</v>
@@ -3316,7 +3330,7 @@
         <v>126</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>42</v>
@@ -3334,7 +3348,7 @@
         <v>53</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>48</v>
@@ -3343,10 +3357,10 @@
         <v>125</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
switch H and M
</commit_message>
<xml_diff>
--- a/TSP.xlsx
+++ b/TSP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/156a5e04750dab24/桌面/TSP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{84FDFF2F-C4A7-4E60-B612-76B73EDBDAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{427E4BFE-2EAF-4964-8938-08E6ECACBF23}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{84FDFF2F-C4A7-4E60-B612-76B73EDBDAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D7927E9-5024-4626-839C-E4BE93248601}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2306,7 +2306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2483,6 +2483,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2783,9 +2786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2844,8 +2845,8 @@
       <c r="F3" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="H3" s="33" t="s">
-        <v>146</v>
+      <c r="H3" s="32" t="s">
+        <v>56</v>
       </c>
       <c r="I3" s="33" t="s">
         <v>42</v>
@@ -2881,8 +2882,8 @@
       <c r="H4" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="I4" s="32" t="s">
-        <v>56</v>
+      <c r="I4" s="33" t="s">
+        <v>146</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -3137,8 +3138,8 @@
       <c r="F19" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="H19" s="33" t="s">
-        <v>146</v>
+      <c r="H19" s="32" t="s">
+        <v>56</v>
       </c>
       <c r="I19" s="33" t="s">
         <v>42</v>
@@ -3170,8 +3171,8 @@
       <c r="H20" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="I20" s="32" t="s">
-        <v>56</v>
+      <c r="I20" s="33" t="s">
+        <v>146</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -3233,8 +3234,8 @@
       <c r="F24" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="H24" s="33" t="s">
-        <v>146</v>
+      <c r="H24" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>42</v>
@@ -3266,8 +3267,8 @@
       <c r="H25" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>56</v>
+      <c r="I25" s="33" t="s">
+        <v>146</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -3330,7 +3331,7 @@
         <v>126</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>42</v>
@@ -3362,8 +3363,8 @@
       <c r="H30" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>56</v>
+      <c r="I30" s="60" t="s">
+        <v>146</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>

</xml_diff>

<commit_message>
xlsx to 100% scale
</commit_message>
<xml_diff>
--- a/TSP.xlsx
+++ b/TSP.xlsx
@@ -2306,7 +2306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2485,9 +2485,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2518,6 +2515,10 @@
 </file>
 
 <file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -3363,7 +3364,7 @@
       <c r="H30" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="I30" s="60" t="s">
+      <c r="I30" s="9" t="s">
         <v>146</v>
       </c>
       <c r="J30" s="9"/>
@@ -3386,7 +3387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCBF856-E901-4FA8-8D9A-D2CBEFF1B64F}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3597,7 +3598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F914A85F-D6ED-45CC-9F6C-6023A3372693}">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update readme; fix bug; update image
</commit_message>
<xml_diff>
--- a/TSP.xlsx
+++ b/TSP.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Program Devs\TSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB6AE34-ED8E-4D4D-A636-44E062F4CA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C0493D-EEE3-4783-8C9C-6BD7C4625A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TSP" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="TSP键位" sheetId="1" r:id="rId1"/>
+    <sheet name="TSP韵母" sheetId="4" r:id="rId2"/>
+    <sheet name="TSP声韵母大全" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$Z$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TSP声韵母大全!$A$1:$Z$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="188">
   <si>
     <t>韵母</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -264,14 +264,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>黄色：a主韵腹</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>绿色：其他</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ua</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -441,14 +433,6 @@
   </si>
   <si>
     <t>üe, ue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>蓝色：e,i,ê主韵腹</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>功能2 待定</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1108,14 +1092,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>含合口韵母</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>含齐撮韵母</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>i, ɿ, ʅ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1124,10 +1100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>功能1 笔画</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>üê, uai</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1148,256 +1120,169 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">i, </t>
-    </r>
-    <r>
-      <rPr>
+    <t>er,ng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y, ÿ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ÿ</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>见右侧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>开</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>ɿ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
+      </rPr>
+      <t>Ø</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
         <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
+      </rPr>
+      <t>、齐</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>ʅ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
         <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, er</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>aoeê</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>m</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>er,ng</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>齐撮韵母</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>开口韵母</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>合口韵母</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y, ÿ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ÿ</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>L</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>K</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>J</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Z</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>见右侧</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
+      </rPr>
+      <t>、撮Ÿ、合</t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t>开</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Ø</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、齐</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Y</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="1"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、撮Ÿ、合</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>W</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1407,10 +1292,6 @@
   </si>
   <si>
     <t>Ø</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标红：汉语拼音采用真开头模式，与此不同</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1737,11 +1618,279 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>保持黑色：均没有声母</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标蓝：汉语拼音采用伪开头模式，与此相同</t>
+    <t>aoeêmn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>黄色：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>主韵腹</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>蓝色：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>e,i,ê</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>主韵腹</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>绿色：其他</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>功能</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>笔画</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>功能</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>待定</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>开口韵母</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>含齐撮韵母</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>齐撮韵母</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>含合口韵母</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>合口韵母</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>彩色：平舌音翘舌音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>灰色（浅）：零声母与介音声母</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>灰色（深）：额外功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>韵母</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>键盘</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>声母</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>零声母保持黑色：汉语拼音没有声母</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>零声母标红：汉语拼音采用真开头模式，与此不同</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>零声母标蓝：汉语拼音采用伪开头模式，与此相同</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1749,7 +1898,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1759,14 +1908,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1907,23 +2048,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B0F0"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="16">
@@ -2282,9 +2416,126 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2293,61 +2544,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2362,9 +2559,6 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2377,7 +2571,16 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2386,82 +2589,16 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2768,794 +2905,802 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:X30"/>
+  <dimension ref="A2:X30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.77734375" style="27"/>
+    <col min="1" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="24" t="s">
+      <c r="C2" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="28" t="s">
+      <c r="L2" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" s="59" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="K3" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="N3" s="59" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="N4" s="59" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="K2" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="L2" s="29" t="s">
+      <c r="J8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="55" t="s">
+        <v>172</v>
+      </c>
+      <c r="J10" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="K10" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="N11" s="24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="N12" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="61" t="s">
         <v>116</v>
-      </c>
-      <c r="N2" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="O2" s="37"/>
-    </row>
-    <row r="3" spans="2:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="K3" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="9"/>
-      <c r="N3" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="O3" s="37"/>
-    </row>
-    <row r="4" spans="2:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="N4" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="O4" s="37"/>
-    </row>
-    <row r="6" spans="2:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="57" t="s">
-        <v>138</v>
-      </c>
-      <c r="I10" s="58" t="s">
-        <v>126</v>
-      </c>
-      <c r="J10" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="K10" s="57" t="s">
-        <v>165</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="9"/>
-    </row>
-    <row r="12" spans="2:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="15" spans="2:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="N17" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="O17" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="P17" s="27" t="s">
-        <v>134</v>
+      <c r="B17" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="24" t="s">
+      <c r="C18" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="K18" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="F18" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="24" t="s">
+      <c r="L18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="T18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="K18" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="P18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="T18" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="W18" s="9" t="s">
+      <c r="U18" s="2"/>
+      <c r="V18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="X18" s="9"/>
+      <c r="X18" s="2"/>
     </row>
     <row r="19" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="H19" s="28" t="s">
+      <c r="F19" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="29" t="s">
+      <c r="I19" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="J19" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="K19" s="9" t="s">
+      <c r="J19" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L19" s="9"/>
-      <c r="N19" s="9" t="s">
+      <c r="L19" s="2"/>
+      <c r="N19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9" t="s">
+      <c r="O19" s="2"/>
+      <c r="P19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q19" s="9" t="s">
+      <c r="Q19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="R19" s="9"/>
-      <c r="T19" s="9" t="s">
+      <c r="R19" s="2"/>
+      <c r="T19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="U19" s="9" t="s">
+      <c r="U19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="V19" s="9" t="s">
+      <c r="V19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
     </row>
     <row r="20" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="C20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="I20" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="N20" s="9" t="s">
+      <c r="E20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="H20" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="I20" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="N20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="T20" s="9" t="s">
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="U20" s="9" t="s">
+      <c r="U20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
     </row>
     <row r="22" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="N22" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="O22" s="27" t="s">
-        <v>125</v>
+      <c r="B22" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="C23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="K23" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="K23" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="L23" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="N23" s="9" t="s">
+      <c r="L23" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="R23" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9" t="s">
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="W23" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="X23" s="9" t="s">
-        <v>93</v>
+      <c r="W23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="X23" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="9" t="s">
+      <c r="I24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J24" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="K24" s="31" t="s">
+      <c r="J24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K24" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="L24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9" t="s">
+      <c r="L24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="X24" s="9"/>
+      <c r="X24" s="2"/>
     </row>
     <row r="25" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="D25" s="24" t="s">
+      <c r="C25" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="H25" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="I25" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="P25" s="9" t="s">
+      <c r="E25" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="H25" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="I25" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="P25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q25" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="R25" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="T25" s="9" t="s">
+      <c r="Q25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="T25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U25" s="9" t="s">
+      <c r="U25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V25" s="9"/>
-      <c r="W25" s="9"/>
-      <c r="X25" s="9"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
     </row>
     <row r="27" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="27" t="s">
+      <c r="B27" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N27" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="O27" s="27" t="s">
+      <c r="N27" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="O27" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="9" t="s">
+      <c r="C28" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K28" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="F28" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I28" s="28" t="s">
+      <c r="L28" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J28" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="K28" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="L28" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="N28" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
-      <c r="T28" s="9"/>
-      <c r="U28" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="V28" s="9"/>
-      <c r="W28" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="X28" s="9" t="s">
+      <c r="V28" s="2"/>
+      <c r="W28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X28" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="H29" s="9" t="s">
+      <c r="F29" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="I29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J29" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="K29" s="9" t="s">
+      <c r="J29" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9" t="s">
+      <c r="L29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9" t="s">
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="W29" s="9"/>
-      <c r="X29" s="9"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
     </row>
     <row r="30" spans="2:24" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="D30" s="9" t="s">
+      <c r="C30" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="R30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
-      <c r="X30" s="9"/>
+      <c r="E30" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="120" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
@@ -3574,63 +3719,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="A1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>96</v>
+      <c r="F1" s="12" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>99</v>
+        <v>157</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="15" t="s">
-        <v>102</v>
+      <c r="F3" s="14" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -3639,113 +3784,113 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>104</v>
+        <v>99</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>105</v>
+      <c r="A5" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F5" s="15"/>
+        <v>156</v>
+      </c>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" s="19" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
+      <c r="A7" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43"/>
+      <c r="A8" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="46"/>
+      <c r="C9" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>94</v>
+      <c r="A10" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>171</v>
-      </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="46"/>
+        <v>90</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" spans="1:6" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
+      <c r="A11" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3765,7 +3910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F914A85F-D6ED-45CC-9F6C-6023A3372693}">
   <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -3778,11 +3923,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -3808,90 +3953,90 @@
         <v>26</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="Y2" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="Z2" s="22" t="s">
         <v>151</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="Z2" s="35" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
-        <v>71</v>
+      <c r="A3" s="43" t="s">
+        <v>69</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -3988,11 +4133,14 @@
         <v>Øa</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
+      </c>
+      <c r="AA3" s="24" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="3" t="s">
         <v>33</v>
       </c>
@@ -4083,24 +4231,24 @@
         <f>_xlfn.CONCAT(X$2,$B4)</f>
         <v>Sia</v>
       </c>
-      <c r="Y4" s="56" t="str">
+      <c r="Y4" s="23" t="str">
         <f t="shared" ref="Y4:Y42" si="1">_xlfn.CONCAT(Z4,$B4)</f>
         <v>Yia</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AA4" s="59" t="s">
-        <v>166</v>
+        <v>128</v>
+      </c>
+      <c r="AA4" s="24" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="7" t="str">
         <f t="shared" ref="D5:S33" si="2">_xlfn.CONCAT(D$2,$B5)</f>
@@ -4186,16 +4334,16 @@
         <f t="shared" si="3"/>
         <v>Sua</v>
       </c>
-      <c r="Y5" s="56" t="str">
+      <c r="Y5" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Wua</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
@@ -4291,19 +4439,16 @@
         <v>Øo</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="AA6" s="59" t="s">
-        <v>181</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D7" s="7" t="str">
         <f t="shared" ref="D7:V7" si="4">_xlfn.CONCAT(D$2,$B7)</f>
@@ -4389,21 +4534,21 @@
         <f t="shared" si="3"/>
         <v>Sio</v>
       </c>
-      <c r="Y7" s="56" t="str">
+      <c r="Y7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Yio</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4489,16 +4634,16 @@
         <f t="shared" si="3"/>
         <v>Suo</v>
       </c>
-      <c r="Y8" s="56" t="str">
+      <c r="Y8" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Wuo</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -4594,16 +4739,16 @@
         <v>Øe</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D10" s="7" t="str">
         <f t="shared" si="2"/>
@@ -4694,11 +4839,11 @@
         <v>Øê</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="3" t="s">
         <v>46</v>
       </c>
@@ -4789,21 +4934,21 @@
         <f t="shared" si="3"/>
         <v>Siê</v>
       </c>
-      <c r="Y11" s="56" t="str">
+      <c r="Y11" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Yiê</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D12" s="7" t="str">
         <f t="shared" si="2"/>
@@ -4889,19 +5034,19 @@
         <f t="shared" si="3"/>
         <v>Süê</v>
       </c>
-      <c r="Y12" s="60" t="str">
+      <c r="Y12" s="25" t="str">
         <f t="shared" si="1"/>
         <v>Ÿüê</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA12" s="59" t="s">
-        <v>182</v>
+        <v>127</v>
+      </c>
+      <c r="AA12" s="24" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
@@ -4992,18 +5137,18 @@
         <f t="shared" si="3"/>
         <v>Si</v>
       </c>
-      <c r="Y13" s="60" t="str">
+      <c r="Y13" s="25" t="str">
         <f t="shared" si="1"/>
         <v>Yi</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>12</v>
@@ -5098,9 +5243,9 @@
       </c>
     </row>
     <row r="15" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>12</v>
@@ -5195,7 +5340,7 @@
       </c>
     </row>
     <row r="16" spans="1:27" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="3" t="s">
         <v>21</v>
       </c>
@@ -5286,21 +5431,21 @@
         <f t="shared" si="3"/>
         <v>Su</v>
       </c>
-      <c r="Y16" s="60" t="str">
+      <c r="Y16" s="25" t="str">
         <f t="shared" si="1"/>
         <v>Wu</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D17" s="7" t="str">
         <f t="shared" si="2"/>
@@ -5386,21 +5531,21 @@
         <f t="shared" si="3"/>
         <v>Sü</v>
       </c>
-      <c r="Y17" s="60" t="str">
+      <c r="Y17" s="25" t="str">
         <f t="shared" si="1"/>
         <v>Ÿü</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D18" s="7" t="str">
         <f t="shared" si="2"/>
@@ -5491,12 +5636,12 @@
         <v>Øer</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
-        <v>79</v>
+      <c r="A19" s="41" t="s">
+        <v>77</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>51</v>
@@ -5593,16 +5738,16 @@
         <v>Øai</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" s="7" t="str">
         <f t="shared" si="2"/>
@@ -5688,16 +5833,16 @@
         <f t="shared" si="3"/>
         <v>Suai</v>
       </c>
-      <c r="Y20" s="56" t="str">
+      <c r="Y20" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Wuai</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="3" t="s">
         <v>48</v>
       </c>
@@ -5793,16 +5938,16 @@
         <v>Øêi</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D22" s="7" t="str">
         <f t="shared" si="2"/>
@@ -5888,20 +6033,20 @@
         <f t="shared" si="3"/>
         <v>Suêi</v>
       </c>
-      <c r="Y22" s="56" t="str">
+      <c r="Y22" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Wuêi</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
-        <v>80</v>
+      <c r="A23" s="41" t="s">
+        <v>78</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>52</v>
@@ -5995,13 +6140,13 @@
         <v>Øau</v>
       </c>
       <c r="Z23" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>42</v>
@@ -6090,16 +6235,16 @@
         <f t="shared" si="3"/>
         <v>Siau</v>
       </c>
-      <c r="Y24" s="56" t="str">
+      <c r="Y24" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Yiau</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="53"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="3" t="s">
         <v>54</v>
       </c>
@@ -6195,11 +6340,11 @@
         <v>Øou</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="3" t="s">
         <v>44</v>
       </c>
@@ -6290,17 +6435,17 @@
         <f t="shared" si="3"/>
         <v>Siou</v>
       </c>
-      <c r="Y26" s="56" t="str">
+      <c r="Y26" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Yiou</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
-        <v>81</v>
+      <c r="A27" s="41" t="s">
+        <v>79</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>35</v>
@@ -6397,11 +6542,11 @@
         <v>Øan</v>
       </c>
       <c r="Z27" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="3" t="s">
         <v>38</v>
       </c>
@@ -6492,18 +6637,18 @@
         <f t="shared" si="3"/>
         <v>Suan</v>
       </c>
-      <c r="Y28" s="56" t="str">
+      <c r="Y28" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Wuan</v>
       </c>
       <c r="Z28" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="3" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>57</v>
@@ -6592,16 +6737,16 @@
         <f t="shared" si="3"/>
         <v>Süan</v>
       </c>
-      <c r="Y29" s="60" t="str">
+      <c r="Y29" s="25" t="str">
         <f t="shared" si="1"/>
         <v>Ÿüan</v>
       </c>
       <c r="Z29" s="1" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="3" t="s">
         <v>40</v>
       </c>
@@ -6697,16 +6842,16 @@
         <v>Øen</v>
       </c>
       <c r="Z30" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D31" s="7" t="str">
         <f t="shared" si="2"/>
@@ -6792,18 +6937,18 @@
         <f t="shared" si="3"/>
         <v>Suen</v>
       </c>
-      <c r="Y31" s="56" t="str">
+      <c r="Y31" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Wuen</v>
       </c>
       <c r="Z31" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>37</v>
@@ -6892,16 +7037,16 @@
         <f t="shared" si="3"/>
         <v>Siên</v>
       </c>
-      <c r="Y32" s="56" t="str">
+      <c r="Y32" s="23" t="str">
         <f>_xlfn.CONCAT(Z32,$B32)</f>
         <v>Yiên</v>
       </c>
       <c r="Z32" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="3" t="s">
         <v>53</v>
       </c>
@@ -6992,21 +7137,21 @@
         <f t="shared" si="3"/>
         <v>Sin</v>
       </c>
-      <c r="Y33" s="60" t="str">
+      <c r="Y33" s="25" t="str">
         <f t="shared" si="1"/>
         <v>Yin</v>
       </c>
       <c r="Z33" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D34" s="7" t="str">
         <f t="shared" ref="D34:S42" si="8">_xlfn.CONCAT(D$2,$B34)</f>
@@ -7092,17 +7237,17 @@
         <f t="shared" si="3"/>
         <v>Süin</v>
       </c>
-      <c r="Y34" s="60" t="str">
+      <c r="Y34" s="25" t="str">
         <f>_xlfn.CONCAT(Z34,$B34)</f>
         <v>Ÿüin</v>
       </c>
       <c r="Z34" s="1" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="53" t="s">
-        <v>82</v>
+      <c r="A35" s="41" t="s">
+        <v>80</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>36</v>
@@ -7199,16 +7344,16 @@
         <v>Øang</v>
       </c>
       <c r="Z35" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="53"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D36" s="7" t="str">
         <f t="shared" si="8"/>
@@ -7294,21 +7439,21 @@
         <f t="shared" si="3"/>
         <v>Siang</v>
       </c>
-      <c r="Y36" s="56" t="str">
+      <c r="Y36" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Yiang</v>
       </c>
       <c r="Z36" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="53"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D37" s="7" t="str">
         <f t="shared" si="8"/>
@@ -7394,21 +7539,21 @@
         <f t="shared" si="3"/>
         <v>Suang</v>
       </c>
-      <c r="Y37" s="56" t="str">
+      <c r="Y37" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Wuang</v>
       </c>
       <c r="Z37" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="53"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D38" s="7" t="str">
         <f t="shared" si="8"/>
@@ -7499,16 +7644,16 @@
         <v>Øong</v>
       </c>
       <c r="Z38" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="53"/>
+      <c r="A39" s="41"/>
       <c r="B39" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D39" s="7" t="str">
         <f t="shared" si="8"/>
@@ -7594,16 +7739,16 @@
         <f t="shared" si="3"/>
         <v>Siong</v>
       </c>
-      <c r="Y39" s="56" t="str">
+      <c r="Y39" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Yiong</v>
       </c>
       <c r="Z39" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="53"/>
+      <c r="A40" s="41"/>
       <c r="B40" s="3" t="s">
         <v>39</v>
       </c>
@@ -7699,11 +7844,11 @@
         <v>Øeng</v>
       </c>
       <c r="Z40" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="53"/>
+      <c r="A41" s="41"/>
       <c r="B41" s="3" t="s">
         <v>50</v>
       </c>
@@ -7794,16 +7939,16 @@
         <f t="shared" si="3"/>
         <v>Sueng</v>
       </c>
-      <c r="Y41" s="56" t="str">
+      <c r="Y41" s="23" t="str">
         <f t="shared" si="1"/>
         <v>Wueng</v>
       </c>
       <c r="Z41" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="53"/>
+      <c r="A42" s="41"/>
       <c r="B42" s="3" t="s">
         <v>41</v>
       </c>
@@ -7894,12 +8039,12 @@
         <f t="shared" si="3"/>
         <v>Sing</v>
       </c>
-      <c r="Y42" s="60" t="str">
+      <c r="Y42" s="25" t="str">
         <f t="shared" si="1"/>
         <v>Ying</v>
       </c>
       <c r="Z42" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>